<commit_message>
Voorlopig excel bestand Pneu
</commit_message>
<xml_diff>
--- a/src/main/resources/dmn/rangnummerPNEU.xlsx
+++ b/src/main/resources/dmn/rangnummerPNEU.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\han\git\rivm\rvp-business\src\main\resources\dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1563A0D-035C-4B54-B160-7434F2D5D6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE93C6C8-16A1-43F2-9CA2-9BE328BA2FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
-    <sheet name="vaccinatietoestand" sheetId="19" r:id="rId1"/>
+    <sheet name="PNEU" sheetId="19" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">vaccinatietoestand!$A$1:$H$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PNEU!$A$1:$I$1</definedName>
     <definedName name="Boolean">#REF!</definedName>
     <definedName name="Rang">#REF!</definedName>
   </definedNames>
@@ -143,9 +143,6 @@
     <t>vaccinatietoestand</t>
   </si>
   <si>
-    <t>primaire serie</t>
-  </si>
-  <si>
     <t>component</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>&gt;= 2020-01-01</t>
+  </si>
+  <si>
+    <t>"Primaire serie"</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,16 +692,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
@@ -724,7 +724,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>29</v>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>29</v>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>30</v>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>1</v>
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>1</v>
@@ -858,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>1</v>
@@ -869,7 +869,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
@@ -898,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -927,7 +927,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>32</v>
@@ -956,7 +956,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>22</v>
@@ -977,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -985,7 +985,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>22</v>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>23</v>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>1</v>
@@ -1043,7 +1043,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>23</v>
@@ -1072,7 +1072,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>23</v>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>1</v>
@@ -1101,7 +1101,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>23</v>
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>23</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>1</v>
@@ -1159,7 +1159,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>23</v>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>23</v>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>1</v>
@@ -1217,7 +1217,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>23</v>
@@ -1238,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>23</v>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>1</v>
@@ -1275,7 +1275,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>23</v>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>28</v>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>1</v>
@@ -1333,7 +1333,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>28</v>
@@ -1354,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>20</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>1</v>
@@ -1391,7 +1391,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>20</v>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>1</v>
@@ -1420,7 +1420,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>31</v>
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>1</v>
@@ -1456,15 +1456,7 @@
       <c r="I27" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H26" xr:uid="{E6F5C849-6F87-43F5-95D0-3C87BFFFF140}"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G28:G1048576" xr:uid="{CCBA37FB-7BA5-464B-9B54-F06D0E9F1C2E}">
-      <formula1>Boolean</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G27" xr:uid="{1BF9627B-27F7-496C-8C57-CE2E4E70E874}">
-      <formula1>Rang</formula1>
-    </dataValidation>
-  </dataValidations>
+  <autoFilter ref="A1:I1" xr:uid="{76820B41-0AB6-4423-A9B3-20CF85256CA0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
direct na genereren .dmn voor PNEU
</commit_message>
<xml_diff>
--- a/src/main/resources/dmn/rangnummerPNEU.xlsx
+++ b/src/main/resources/dmn/rangnummerPNEU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\han\git\rivm\rvp-business\src\main\resources\dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE93C6C8-16A1-43F2-9CA2-9BE328BA2FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66170845-745A-49EF-9916-520D57B64F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="32040" yWindow="1575" windowWidth="24450" windowHeight="11505" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="PNEU" sheetId="19" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>[214 .. 365)</t>
   </si>
   <si>
-    <t>vaccinatietoestand</t>
-  </si>
-  <si>
     <t>component</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>"Primaire serie"</t>
+  </si>
+  <si>
+    <t>PNEU</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,16 +692,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
@@ -716,7 +716,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>29</v>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>29</v>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>30</v>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>1</v>
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>1</v>
@@ -858,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>1</v>
@@ -869,7 +869,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
@@ -898,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -927,7 +927,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>32</v>
@@ -956,7 +956,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>22</v>
@@ -977,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -985,7 +985,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>22</v>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>23</v>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>1</v>
@@ -1043,7 +1043,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>23</v>
@@ -1072,7 +1072,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>23</v>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>1</v>
@@ -1101,7 +1101,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>23</v>
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>23</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>1</v>
@@ -1159,7 +1159,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>23</v>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>23</v>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>1</v>
@@ -1217,7 +1217,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>23</v>
@@ -1238,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>23</v>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>1</v>
@@ -1275,7 +1275,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>23</v>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>28</v>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>1</v>
@@ -1333,7 +1333,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>28</v>
@@ -1354,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>20</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>1</v>
@@ -1391,7 +1391,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>20</v>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>1</v>
@@ -1420,7 +1420,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>31</v>
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>1</v>

</xml_diff>